<commit_message>
Release 1.5 Aggiunto controllo su adj g2u che controlla le celle 3g
</commit_message>
<xml_diff>
--- a/CDR_SU_PZ162_2G_MODERNIZATION.xlsx
+++ b/CDR_SU_PZ162_2G_MODERNIZATION.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2D373FEE-0823-4983-B13C-2A95C622EEB7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19212" windowHeight="9048" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revision History" sheetId="8" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BTS!$B$1:$AL$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'External 3G cells'!$A$1:$U$13</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autore</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{09E95A4E-CE16-49E9-B0D8-81FD6EC29DA9}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +43,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -53,7 +52,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 create
@@ -62,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6C70E38B-80B7-4D03-A75E-7161438C00C3}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -79,14 +78,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 inserire il codice del BSC</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{62AC555D-CC0D-43BB-B26E-CF35F421B463}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +93,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -103,14 +102,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 inserire il codice cella</t>
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{78BE789C-3E35-41DB-9909-923BCC3596FC}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -134,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{243E4F3E-26A3-4EE9-9FF0-E27FC6F6BF28}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{F5AA91F5-98CC-42CB-8BFF-195CAA9D2E7F}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +167,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -177,7 +176,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 inserire codice LAC.
@@ -186,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{D15319BC-D9B9-4EED-86D8-2148EB9364CB}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +193,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -203,7 +202,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 cell identity
@@ -211,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{095BD31A-3589-4F45-84BB-4E5CA68F5B76}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -235,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{97283C30-55BF-4F80-A7CC-80D66ACE6380}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -243,7 +242,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -252,7 +251,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 base station color code
@@ -260,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{F4EE4DBC-FD3C-4131-B3B2-5EC2065498DC}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -268,7 +267,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -277,14 +276,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 frequenza BCCH da tool planning</t>
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{41B16F3E-E9AA-46A8-9CA7-62317AA737BF}">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +291,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -301,14 +300,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 channel group 0 sempre presente</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{190711E5-8C92-43C1-BF0B-B64ACEFB3C97}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -316,7 +315,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -325,14 +324,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 sempre pari a 1</t>
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{19F293BE-B90E-4564-89BD-CDE85E567FDB}">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -357,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{9471864B-C455-4AD8-9815-4E0B64305EEB}">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -381,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{8DEE242A-BA41-49AF-87D3-C126979FD534}">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{A6CAC701-4F60-49DB-A713-44147897FE56}">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -413,7 +412,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -422,14 +421,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 uguale a BSPWRT</t>
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{EB637269-A04B-4C12-B97C-5482327DF426}">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -453,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{5739E9CC-D0AD-452A-94CA-EA04D1F4D6E1}">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -478,7 +477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{A1C39896-239A-4C97-8E74-256515CE0F2F}">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -503,7 +502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{3901CBD5-0EF1-410E-9015-428117D6D781}">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -529,7 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{7DBC1646-5119-4DDA-AB99-773DBFD3BE00}">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -553,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{3DDA75ED-8654-4D91-8ECB-93003DF9D13A}">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -577,7 +576,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{30E7914E-6CE8-41F0-BC48-9F9CDA6B13D5}">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -585,7 +584,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -594,14 +593,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Numero di TRX sulla cella - 1 (ossia solo i TRX di TCH)</t>
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{262B6031-8EC6-4279-B64C-AC87AB8196DE}">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -609,7 +608,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -618,14 +617,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 mettere SY se il chgroup 1 è definito. Altrimenti lasciare vuoto</t>
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{977C61E5-B175-4F23-9FB9-41706575AF74}">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -650,7 +649,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -679,7 +678,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{C0ABE016-DD7E-49A8-9898-E20025D28B5F}">
+    <comment ref="AB1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -687,7 +686,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -696,14 +695,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Hopping sequence number</t>
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{6B9D2E90-AFDF-4BE7-9F3B-01BFCD14EC9C}">
+    <comment ref="AC1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -711,7 +710,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -720,14 +719,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 MAIO del TRX 1 del chgroup</t>
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{A8841E49-8983-4F4D-A205-CE909EE83D8C}">
+    <comment ref="AD1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -735,7 +734,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -744,14 +743,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 maio del TRX 2 del CHGROUP 1</t>
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{86A5B155-6791-4F1C-8ED2-617DFE825DA1}">
+    <comment ref="AE1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -759,7 +758,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -768,14 +767,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 maio del TRX3 del chgroup</t>
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{1B0EFB5D-A658-4503-B880-754D2ED4CBFA}">
+    <comment ref="AF1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -783,7 +782,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -792,14 +791,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 frequenze su cui hoppano i TRX di traffico</t>
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{A29EC5A3-6834-44F5-A067-B22F04CE28A5}">
+    <comment ref="AL1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -807,7 +806,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -816,7 +815,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 se le celle devono rimanre bloccate inserire keep_lockd tramite menù a tendina</t>
@@ -828,12 +827,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autore</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{98CC34D1-3F88-4515-AD78-746BCE369A3A}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -841,7 +840,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autore:</t>
         </r>
@@ -850,14 +849,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 non si definiscono le celle P e Q. </t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E0133400-23A0-478A-A245-0887A885648B}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -881,7 +880,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{AE776EAD-FFDC-4DA8-AD7C-24A0AC4B034F}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -905,7 +904,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{90F465D5-4DB0-4065-A444-59287CCB7B76}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -929,7 +928,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{9071C90E-EC92-4AAF-A835-19C2046BB4AB}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -953,7 +952,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{19C1A620-0204-4B73-A409-3E30F68DEDC1}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -977,7 +976,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{EEE2D3E1-97F9-43D0-B4FA-596ECBD45F7C}">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1001,7 +1000,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{475F664D-DF7F-466D-8B65-ABF428513B2F}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1026,7 +1025,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{F8F14C4D-AC1C-4A1C-BB98-10B9CB27A1FE}">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1050,7 +1049,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{67368307-C466-4112-B32C-31F472AC3E26}">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1074,7 +1073,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{9611EDA6-5F09-4739-B638-0986AE2303EF}">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1098,7 +1097,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{61664B93-0530-491C-9043-599790E0DB0A}">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1122,7 +1121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{C0A3375F-E644-45F8-AD72-DFCEB85CB14D}">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1146,7 +1145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{165478F0-586D-4C2B-8716-35B6CC175A8D}">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1528,14 +1527,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_)"/>
-    <numFmt numFmtId="166" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;L.&quot;\ * #,##0_-;\-&quot;L.&quot;\ * #,##0_-;_-&quot;L.&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_)"/>
+    <numFmt numFmtId="165" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;L.&quot;\ * #,##0_-;\-&quot;L.&quot;\ * #,##0_-;_-&quot;L.&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="53">
+  <fonts count="51">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1876,19 +1875,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="62">
@@ -2536,7 +2522,7 @@
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2560,16 +2546,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="47" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="47" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
@@ -2819,267 +2805,267 @@
     </xf>
   </cellXfs>
   <cellStyles count="261">
-    <cellStyle name="_x000a_shell=progma" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="_x000a_shell=progma 2" xfId="96" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="_x000a_shell=progma 2 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="_x000a_shell=progma 2 2 2" xfId="164" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="_x000a_shell=progma 3" xfId="102" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="_x000a_shell=progma_CDR_TP_W10_B_Rbs_PA2" xfId="101" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="%" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="% 14" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="% 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="% 2 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="% 7" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="%_Asignacion RNCs MAN MALAGA 2011 S.21" xfId="10" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="%_BASICO 7.2 PLANTILLA DATOS RADIO nueva integración  SIN DATOS TX 2300291 ANDUJAR MIRANDA" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="%_DATOS RADIO AMP PORT MEDIO 7.2 400479 HUERCAL OVERA CUARTEL -b" xfId="12" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="%_MA12012602-DATOS RADIO AMP PORT MEDIO 7.2 2900146 ALMOGIA EB" xfId="13" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="%_MA12021301_DATOS RADIO AMP PORT M 7.2-B 7.2 2900174 OJENv2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="%_Masterlist" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="%_Masterlist 2" xfId="93" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="%_Plantilla_datos_radio_conf2012_v10 (2)" xfId="16" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="%_Plantilla_datos_radio_conf2012_v2" xfId="17" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="_DATOS RNC UMTS-020806" xfId="18" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="_SAC_generar_el_archivo_en_Provincia" xfId="19" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="_UMTS-AREATZA_3G-3G3G-2G" xfId="20" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="_VARIOS_2011_05_25" xfId="21" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="_VARIOS_2011_05_25_GOAM 1P" xfId="22" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="_X_template_I.P_v1" xfId="23" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_" xfId="24" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="20% - Accent1 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="20% - Accent1 3" xfId="221" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="20% - Accent1 4" xfId="187" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="20% - Accent1 5" xfId="246" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="20% - Accent2 3" xfId="220" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="20% - Accent2 4" xfId="186" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="20% - Accent2 5" xfId="249" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="20% - Accent3 3" xfId="219" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="20% - Accent3 4" xfId="185" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="20% - Accent3 5" xfId="250" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="20% - Accent4 3" xfId="218" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="20% - Accent4 4" xfId="184" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="20% - Accent4 5" xfId="254" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="20% - Accent5 3" xfId="130" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="20% - Accent5 4" xfId="217" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="20% - Accent5 5" xfId="183" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="20% - Accent6 3" xfId="216" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="20% - Accent6 4" xfId="182" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="20% - Accent6 5" xfId="257" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="_x000a_shell=progma" xfId="4"/>
+    <cellStyle name="_x000a_shell=progma 2" xfId="96"/>
+    <cellStyle name="_x000a_shell=progma 2 2" xfId="98"/>
+    <cellStyle name="_x000a_shell=progma 2 2 2" xfId="164"/>
+    <cellStyle name="_x000a_shell=progma 3" xfId="102"/>
+    <cellStyle name="_x000a_shell=progma_CDR_TP_W10_B_Rbs_PA2" xfId="101"/>
+    <cellStyle name="%" xfId="5"/>
+    <cellStyle name="% 14" xfId="6"/>
+    <cellStyle name="% 2" xfId="7"/>
+    <cellStyle name="% 2 2 2" xfId="8"/>
+    <cellStyle name="% 7" xfId="9"/>
+    <cellStyle name="%_Asignacion RNCs MAN MALAGA 2011 S.21" xfId="10"/>
+    <cellStyle name="%_BASICO 7.2 PLANTILLA DATOS RADIO nueva integración  SIN DATOS TX 2300291 ANDUJAR MIRANDA" xfId="11"/>
+    <cellStyle name="%_DATOS RADIO AMP PORT MEDIO 7.2 400479 HUERCAL OVERA CUARTEL -b" xfId="12"/>
+    <cellStyle name="%_MA12012602-DATOS RADIO AMP PORT MEDIO 7.2 2900146 ALMOGIA EB" xfId="13"/>
+    <cellStyle name="%_MA12021301_DATOS RADIO AMP PORT M 7.2-B 7.2 2900174 OJENv2" xfId="14"/>
+    <cellStyle name="%_Masterlist" xfId="15"/>
+    <cellStyle name="%_Masterlist 2" xfId="93"/>
+    <cellStyle name="%_Plantilla_datos_radio_conf2012_v10 (2)" xfId="16"/>
+    <cellStyle name="%_Plantilla_datos_radio_conf2012_v2" xfId="17"/>
+    <cellStyle name="_DATOS RNC UMTS-020806" xfId="18"/>
+    <cellStyle name="_SAC_generar_el_archivo_en_Provincia" xfId="19"/>
+    <cellStyle name="_UMTS-AREATZA_3G-3G3G-2G" xfId="20"/>
+    <cellStyle name="_VARIOS_2011_05_25" xfId="21"/>
+    <cellStyle name="_VARIOS_2011_05_25_GOAM 1P" xfId="22"/>
+    <cellStyle name="_X_template_I.P_v1" xfId="23"/>
+    <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_" xfId="24"/>
+    <cellStyle name="20% - Accent1 2" xfId="25"/>
+    <cellStyle name="20% - Accent1 3" xfId="221"/>
+    <cellStyle name="20% - Accent1 4" xfId="187"/>
+    <cellStyle name="20% - Accent1 5" xfId="246"/>
+    <cellStyle name="20% - Accent2 2" xfId="26"/>
+    <cellStyle name="20% - Accent2 3" xfId="220"/>
+    <cellStyle name="20% - Accent2 4" xfId="186"/>
+    <cellStyle name="20% - Accent2 5" xfId="249"/>
+    <cellStyle name="20% - Accent3 2" xfId="27"/>
+    <cellStyle name="20% - Accent3 3" xfId="219"/>
+    <cellStyle name="20% - Accent3 4" xfId="185"/>
+    <cellStyle name="20% - Accent3 5" xfId="250"/>
+    <cellStyle name="20% - Accent4 2" xfId="28"/>
+    <cellStyle name="20% - Accent4 3" xfId="218"/>
+    <cellStyle name="20% - Accent4 4" xfId="184"/>
+    <cellStyle name="20% - Accent4 5" xfId="254"/>
+    <cellStyle name="20% - Accent5 2" xfId="34"/>
+    <cellStyle name="20% - Accent5 3" xfId="130"/>
+    <cellStyle name="20% - Accent5 4" xfId="217"/>
+    <cellStyle name="20% - Accent5 5" xfId="183"/>
+    <cellStyle name="20% - Accent6 2" xfId="29"/>
+    <cellStyle name="20% - Accent6 3" xfId="216"/>
+    <cellStyle name="20% - Accent6 4" xfId="182"/>
+    <cellStyle name="20% - Accent6 5" xfId="257"/>
     <cellStyle name="20% - Colore 1" xfId="129" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Colore 2" xfId="128" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Colore 3" xfId="127" builtinId="38" customBuiltin="1"/>
     <cellStyle name="20% - Colore 4" xfId="126" builtinId="42" customBuiltin="1"/>
     <cellStyle name="20% - Colore 5" xfId="125" builtinId="46" customBuiltin="1"/>
     <cellStyle name="20% - Colore 6" xfId="124" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis1 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="20% - Énfasis2 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="20% - Énfasis3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="20% - Énfasis4 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="20% - Énfasis6 2" xfId="35" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="36" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="40% - Accent1 3" xfId="215" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="40% - Accent1 4" xfId="181" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="40% - Accent1 5" xfId="247" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="40% - Accent2 3" xfId="123" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="40% - Accent2 4" xfId="214" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="40% - Accent2 5" xfId="180" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="40% - Accent3 3" xfId="213" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="40% - Accent3 4" xfId="179" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="40% - Accent3 5" xfId="251" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="40% - Accent4 3" xfId="212" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="40% - Accent4 4" xfId="178" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="40% - Accent4 5" xfId="255" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="40% - Accent5 3" xfId="122" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="40% - Accent5 4" xfId="211" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="40% - Accent5 5" xfId="177" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="39" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="40% - Accent6 3" xfId="210" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="40% - Accent6 4" xfId="176" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="40% - Accent6 5" xfId="258" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="20% - Énfasis1 2" xfId="30"/>
+    <cellStyle name="20% - Énfasis2 2" xfId="31"/>
+    <cellStyle name="20% - Énfasis3 2" xfId="32"/>
+    <cellStyle name="20% - Énfasis4 2" xfId="33"/>
+    <cellStyle name="20% - Énfasis6 2" xfId="35"/>
+    <cellStyle name="40% - Accent1 2" xfId="36"/>
+    <cellStyle name="40% - Accent1 3" xfId="215"/>
+    <cellStyle name="40% - Accent1 4" xfId="181"/>
+    <cellStyle name="40% - Accent1 5" xfId="247"/>
+    <cellStyle name="40% - Accent2 2" xfId="41"/>
+    <cellStyle name="40% - Accent2 3" xfId="123"/>
+    <cellStyle name="40% - Accent2 4" xfId="214"/>
+    <cellStyle name="40% - Accent2 5" xfId="180"/>
+    <cellStyle name="40% - Accent3 2" xfId="37"/>
+    <cellStyle name="40% - Accent3 3" xfId="213"/>
+    <cellStyle name="40% - Accent3 4" xfId="179"/>
+    <cellStyle name="40% - Accent3 5" xfId="251"/>
+    <cellStyle name="40% - Accent4 2" xfId="38"/>
+    <cellStyle name="40% - Accent4 3" xfId="212"/>
+    <cellStyle name="40% - Accent4 4" xfId="178"/>
+    <cellStyle name="40% - Accent4 5" xfId="255"/>
+    <cellStyle name="40% - Accent5 2" xfId="44"/>
+    <cellStyle name="40% - Accent5 3" xfId="122"/>
+    <cellStyle name="40% - Accent5 4" xfId="211"/>
+    <cellStyle name="40% - Accent5 5" xfId="177"/>
+    <cellStyle name="40% - Accent6 2" xfId="39"/>
+    <cellStyle name="40% - Accent6 3" xfId="210"/>
+    <cellStyle name="40% - Accent6 4" xfId="176"/>
+    <cellStyle name="40% - Accent6 5" xfId="258"/>
     <cellStyle name="40% - Colore 1" xfId="121" builtinId="31" customBuiltin="1"/>
     <cellStyle name="40% - Colore 2" xfId="120" builtinId="35" customBuiltin="1"/>
     <cellStyle name="40% - Colore 3" xfId="119" builtinId="39" customBuiltin="1"/>
     <cellStyle name="40% - Colore 4" xfId="118" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Colore 5" xfId="117" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Colore 6" xfId="116" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1 2" xfId="40" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="40% - Énfasis3 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="40% - Énfasis4 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="40% - Énfasis6 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="60% - Accent1 3" xfId="209" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="60% - Accent1 4" xfId="175" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="60% - Accent1 5" xfId="248" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="60% - Accent2 3" xfId="115" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="60% - Accent2 4" xfId="208" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="60% - Accent2 5" xfId="174" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="60% - Accent3 3" xfId="207" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="60% - Accent3 4" xfId="173" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="60% - Accent3 5" xfId="252" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="60% - Accent4 3" xfId="206" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="60% - Accent4 4" xfId="172" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="60% - Accent4 5" xfId="256" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="60% - Accent5 3" xfId="114" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="60% - Accent5 4" xfId="205" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="60% - Accent5 5" xfId="171" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="60% - Accent6 3" xfId="222" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="60% - Accent6 4" xfId="188" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="60% - Accent6 5" xfId="259" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="40% - Énfasis1 2" xfId="40"/>
+    <cellStyle name="40% - Énfasis3 2" xfId="42"/>
+    <cellStyle name="40% - Énfasis4 2" xfId="43"/>
+    <cellStyle name="40% - Énfasis6 2" xfId="45"/>
+    <cellStyle name="60% - Accent1 2" xfId="46"/>
+    <cellStyle name="60% - Accent1 3" xfId="209"/>
+    <cellStyle name="60% - Accent1 4" xfId="175"/>
+    <cellStyle name="60% - Accent1 5" xfId="248"/>
+    <cellStyle name="60% - Accent2 2" xfId="51"/>
+    <cellStyle name="60% - Accent2 3" xfId="115"/>
+    <cellStyle name="60% - Accent2 4" xfId="208"/>
+    <cellStyle name="60% - Accent2 5" xfId="174"/>
+    <cellStyle name="60% - Accent3 2" xfId="47"/>
+    <cellStyle name="60% - Accent3 3" xfId="207"/>
+    <cellStyle name="60% - Accent3 4" xfId="173"/>
+    <cellStyle name="60% - Accent3 5" xfId="252"/>
+    <cellStyle name="60% - Accent4 2" xfId="48"/>
+    <cellStyle name="60% - Accent4 3" xfId="206"/>
+    <cellStyle name="60% - Accent4 4" xfId="172"/>
+    <cellStyle name="60% - Accent4 5" xfId="256"/>
+    <cellStyle name="60% - Accent5 2" xfId="54"/>
+    <cellStyle name="60% - Accent5 3" xfId="114"/>
+    <cellStyle name="60% - Accent5 4" xfId="205"/>
+    <cellStyle name="60% - Accent5 5" xfId="171"/>
+    <cellStyle name="60% - Accent6 2" xfId="49"/>
+    <cellStyle name="60% - Accent6 3" xfId="222"/>
+    <cellStyle name="60% - Accent6 4" xfId="188"/>
+    <cellStyle name="60% - Accent6 5" xfId="259"/>
     <cellStyle name="60% - Colore 1" xfId="113" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Colore 2" xfId="112" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Colore 3" xfId="111" builtinId="40" customBuiltin="1"/>
     <cellStyle name="60% - Colore 4" xfId="110" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Colore 5" xfId="109" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Colore 6" xfId="131" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="60% - Énfasis3 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="60% - Énfasis4 2" xfId="53" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="60% - Énfasis6 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Accent1 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Accent1 3" xfId="223" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Accent1 4" xfId="189" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Accent1 5" xfId="245" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
-    <cellStyle name="Accent2 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Accent2 3" xfId="132" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Accent2 4" xfId="224" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Accent2 5" xfId="190" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Accent3 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Accent3 3" xfId="133" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Accent3 4" xfId="225" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Accent3 5" xfId="191" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Accent4 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Accent4 3" xfId="226" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Accent4 4" xfId="192" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Accent4 5" xfId="253" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
-    <cellStyle name="Accent5 2" xfId="69" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Accent5 3" xfId="134" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Accent5 4" xfId="227" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Accent5 5" xfId="193" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Accent6 2" xfId="70" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Accent6 3" xfId="135" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Accent6 4" xfId="228" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Accent6 5" xfId="194" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Bad 2" xfId="76" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Bad 3" xfId="136" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Bad 4" xfId="237" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Bad 5" xfId="203" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Buena 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Calcolo" xfId="165" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Calculation 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Cálculo 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Celda de comprobación 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Celda vinculada 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Cella collegata" xfId="166" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Cella da controllare" xfId="167" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Check Cell 2" xfId="137" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="60% - Énfasis1 2" xfId="50"/>
+    <cellStyle name="60% - Énfasis3 2" xfId="52"/>
+    <cellStyle name="60% - Énfasis4 2" xfId="53"/>
+    <cellStyle name="60% - Énfasis6 2" xfId="55"/>
+    <cellStyle name="Accent1 2" xfId="56"/>
+    <cellStyle name="Accent1 3" xfId="223"/>
+    <cellStyle name="Accent1 4" xfId="189"/>
+    <cellStyle name="Accent1 5" xfId="245"/>
+    <cellStyle name="Accent2 2" xfId="66"/>
+    <cellStyle name="Accent2 3" xfId="132"/>
+    <cellStyle name="Accent2 4" xfId="224"/>
+    <cellStyle name="Accent2 5" xfId="190"/>
+    <cellStyle name="Accent3 2" xfId="67"/>
+    <cellStyle name="Accent3 3" xfId="133"/>
+    <cellStyle name="Accent3 4" xfId="225"/>
+    <cellStyle name="Accent3 5" xfId="191"/>
+    <cellStyle name="Accent4 2" xfId="57"/>
+    <cellStyle name="Accent4 3" xfId="226"/>
+    <cellStyle name="Accent4 4" xfId="192"/>
+    <cellStyle name="Accent4 5" xfId="253"/>
+    <cellStyle name="Accent5 2" xfId="69"/>
+    <cellStyle name="Accent5 3" xfId="134"/>
+    <cellStyle name="Accent5 4" xfId="227"/>
+    <cellStyle name="Accent5 5" xfId="193"/>
+    <cellStyle name="Accent6 2" xfId="70"/>
+    <cellStyle name="Accent6 3" xfId="135"/>
+    <cellStyle name="Accent6 4" xfId="228"/>
+    <cellStyle name="Accent6 5" xfId="194"/>
+    <cellStyle name="Bad 2" xfId="76"/>
+    <cellStyle name="Bad 3" xfId="136"/>
+    <cellStyle name="Bad 4" xfId="237"/>
+    <cellStyle name="Bad 5" xfId="203"/>
+    <cellStyle name="Buena 2" xfId="58"/>
+    <cellStyle name="Calcolo" xfId="165"/>
+    <cellStyle name="Calculation 2" xfId="59"/>
+    <cellStyle name="Cálculo 2" xfId="60"/>
+    <cellStyle name="Celda de comprobación 2" xfId="61"/>
+    <cellStyle name="Celda vinculada 2" xfId="62"/>
+    <cellStyle name="Cella collegata" xfId="166"/>
+    <cellStyle name="Cella da controllare" xfId="167"/>
+    <cellStyle name="Check Cell 2" xfId="137"/>
     <cellStyle name="Colore 1" xfId="138" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Colore 2" xfId="139" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Colore 3" xfId="140" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Colore 4" xfId="141" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Colore 5" xfId="142" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Colore 6" xfId="143" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="edlsfjk" xfId="63" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Encabezado 4 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Énfasis1 2" xfId="65" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Énfasis4 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Entrada 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Estilo 1" xfId="72" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Euro" xfId="73" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Euro 2" xfId="95" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Explanatory Text 3" xfId="144" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Explanatory Text 4" xfId="230" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
-    <cellStyle name="Explanatory Text 5" xfId="196" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
-    <cellStyle name="Good 2" xfId="145" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Good 3" xfId="238" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
-    <cellStyle name="Good 4" xfId="204" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
-    <cellStyle name="Good 5" xfId="244" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
-    <cellStyle name="Heading 1 2" xfId="146" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Heading 1 3" xfId="232" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
-    <cellStyle name="Heading 1 4" xfId="198" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
-    <cellStyle name="Heading 1 5" xfId="240" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
-    <cellStyle name="Heading 2 2" xfId="74" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Heading 2 3" xfId="233" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="Heading 2 4" xfId="199" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
-    <cellStyle name="Heading 2 5" xfId="241" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
-    <cellStyle name="Heading 3 2" xfId="75" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Heading 3 3" xfId="234" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
-    <cellStyle name="Heading 3 4" xfId="200" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="Heading 3 5" xfId="242" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
-    <cellStyle name="Heading 4 2" xfId="147" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Heading 4 3" xfId="235" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
-    <cellStyle name="Heading 4 4" xfId="201" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
-    <cellStyle name="Heading 4 5" xfId="243" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="edlsfjk" xfId="63"/>
+    <cellStyle name="Encabezado 4 2" xfId="64"/>
+    <cellStyle name="Énfasis1 2" xfId="65"/>
+    <cellStyle name="Énfasis4 2" xfId="68"/>
+    <cellStyle name="Entrada 2" xfId="71"/>
+    <cellStyle name="Estilo 1" xfId="72"/>
+    <cellStyle name="Euro" xfId="73"/>
+    <cellStyle name="Euro 2" xfId="95"/>
+    <cellStyle name="Explanatory Text 2" xfId="86"/>
+    <cellStyle name="Explanatory Text 3" xfId="144"/>
+    <cellStyle name="Explanatory Text 4" xfId="230"/>
+    <cellStyle name="Explanatory Text 5" xfId="196"/>
+    <cellStyle name="Good 2" xfId="145"/>
+    <cellStyle name="Good 3" xfId="238"/>
+    <cellStyle name="Good 4" xfId="204"/>
+    <cellStyle name="Good 5" xfId="244"/>
+    <cellStyle name="Heading 1 2" xfId="146"/>
+    <cellStyle name="Heading 1 3" xfId="232"/>
+    <cellStyle name="Heading 1 4" xfId="198"/>
+    <cellStyle name="Heading 1 5" xfId="240"/>
+    <cellStyle name="Heading 2 2" xfId="74"/>
+    <cellStyle name="Heading 2 3" xfId="233"/>
+    <cellStyle name="Heading 2 4" xfId="199"/>
+    <cellStyle name="Heading 2 5" xfId="241"/>
+    <cellStyle name="Heading 3 2" xfId="75"/>
+    <cellStyle name="Heading 3 3" xfId="234"/>
+    <cellStyle name="Heading 3 4" xfId="200"/>
+    <cellStyle name="Heading 3 5" xfId="242"/>
+    <cellStyle name="Heading 4 2" xfId="147"/>
+    <cellStyle name="Heading 4 3" xfId="235"/>
+    <cellStyle name="Heading 4 4" xfId="201"/>
+    <cellStyle name="Heading 4 5" xfId="243"/>
     <cellStyle name="Input" xfId="2" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Input 2" xfId="148" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Jun" xfId="97" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="149" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Migliaia (0)_app2" xfId="99" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Neutral 2" xfId="77" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Neutral 3" xfId="150" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Neutral 4" xfId="229" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="Neutral 5" xfId="195" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Input 2" xfId="148"/>
+    <cellStyle name="Jun" xfId="97"/>
+    <cellStyle name="Linked Cell 2" xfId="149"/>
+    <cellStyle name="Migliaia (0)_app2" xfId="99"/>
+    <cellStyle name="Neutral 2" xfId="77"/>
+    <cellStyle name="Neutral 3" xfId="150"/>
+    <cellStyle name="Neutral 4" xfId="229"/>
+    <cellStyle name="Neutral 5" xfId="195"/>
     <cellStyle name="Neutrale" xfId="151" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Normal 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Normal 3 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Normal 4" xfId="100" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Normal 4 2" xfId="170" xr:uid="{5A9301B8-F7AD-4C35-82F1-1EB5A67B1ECB}"/>
+    <cellStyle name="Normal 2" xfId="78"/>
+    <cellStyle name="Normal 2 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="79"/>
+    <cellStyle name="Normal 3 2" xfId="94"/>
+    <cellStyle name="Normal 4" xfId="100"/>
+    <cellStyle name="Normal 4 2" xfId="170"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Normale 2" xfId="108" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Normale 4" xfId="106" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Normale_CDR_Wind_Project_Roma_revH_6_0_fogli radio 2" xfId="260" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Nota" xfId="169" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Nota 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Nota 2 2" xfId="107" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Notas 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Note 2" xfId="152" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="nteb" xfId="81" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Normale 2" xfId="108"/>
+    <cellStyle name="Normale 4" xfId="106"/>
+    <cellStyle name="Normale_CDR_Wind_Project_Roma_revH_6_0_fogli radio 2" xfId="260"/>
+    <cellStyle name="Nota" xfId="169"/>
+    <cellStyle name="Nota 2" xfId="103"/>
+    <cellStyle name="Nota 2 2" xfId="107"/>
+    <cellStyle name="Notas 2" xfId="80"/>
+    <cellStyle name="Note 2" xfId="152"/>
+    <cellStyle name="nteb" xfId="81"/>
     <cellStyle name="Output" xfId="3" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Output 2" xfId="82" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="Salida 2" xfId="83" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="Style 1" xfId="84" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="Style 1 2" xfId="105" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="Testo avviso" xfId="168" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Output 2" xfId="82"/>
+    <cellStyle name="Salida 2" xfId="83"/>
+    <cellStyle name="Style 1" xfId="84"/>
+    <cellStyle name="Style 1 2" xfId="105"/>
+    <cellStyle name="Testo avviso" xfId="168"/>
     <cellStyle name="Testo descrittivo" xfId="153" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia 2" xfId="85" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="Title 2" xfId="87" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="Title 3" xfId="231" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
-    <cellStyle name="Title 4" xfId="197" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
-    <cellStyle name="Title 5" xfId="239" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Texto de advertencia 2" xfId="85"/>
+    <cellStyle name="Title 2" xfId="87"/>
+    <cellStyle name="Title 3" xfId="231"/>
+    <cellStyle name="Title 4" xfId="197"/>
+    <cellStyle name="Title 5" xfId="239"/>
     <cellStyle name="Titolo" xfId="154" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Titolo 1" xfId="155" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Titolo 2" xfId="156" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Titolo 3" xfId="157" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Titolo 4" xfId="158" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Título 1 2" xfId="88" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="Título 2 2" xfId="89" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="Título 3 2" xfId="90" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="Título 4" xfId="91" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
-    <cellStyle name="Total 2" xfId="92" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
-    <cellStyle name="Total 3" xfId="159" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
-    <cellStyle name="Total 4" xfId="236" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
-    <cellStyle name="Total 5" xfId="202" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="Título 1 2" xfId="88"/>
+    <cellStyle name="Título 2 2" xfId="89"/>
+    <cellStyle name="Título 3 2" xfId="90"/>
+    <cellStyle name="Título 4" xfId="91"/>
+    <cellStyle name="Total 2" xfId="92"/>
+    <cellStyle name="Total 3" xfId="159"/>
+    <cellStyle name="Total 4" xfId="236"/>
+    <cellStyle name="Total 5" xfId="202"/>
     <cellStyle name="Totale" xfId="160" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Valore non valido" xfId="161" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Valore valido" xfId="162" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Valuta (0)_app2" xfId="104" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
-    <cellStyle name="Warning Text 2" xfId="163" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Valuta (0)_app2" xfId="104"/>
+    <cellStyle name="Warning Text 2" xfId="163"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3356,18 +3342,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CB59D5-B298-4AEE-8D5D-8CB9C163BBFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="77.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="77.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3418,46 +3404,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E14" sqref="E14"/>
+      <pane xSplit="3" topLeftCell="AE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="7" width="15.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="7" width="15.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.44140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.44140625" customWidth="1"/>
-    <col min="17" max="17" width="18.33203125" customWidth="1"/>
-    <col min="18" max="18" width="14.5546875" style="26" customWidth="1"/>
-    <col min="19" max="19" width="17.5546875" style="26" customWidth="1"/>
-    <col min="20" max="22" width="18.33203125" style="3" customWidth="1"/>
-    <col min="23" max="23" width="28.44140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.44140625" style="26" customWidth="1"/>
-    <col min="25" max="25" width="16.88671875" style="26" customWidth="1"/>
-    <col min="26" max="26" width="22.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.6640625" customWidth="1"/>
-    <col min="29" max="29" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="23.44140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.6640625" customWidth="1"/>
-    <col min="37" max="37" width="20.33203125" customWidth="1"/>
-    <col min="38" max="38" width="26.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" style="26" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" style="26" customWidth="1"/>
+    <col min="20" max="22" width="18.28515625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="28.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.42578125" style="26" customWidth="1"/>
+    <col min="25" max="25" width="16.85546875" style="26" customWidth="1"/>
+    <col min="26" max="26" width="22.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.7109375" customWidth="1"/>
+    <col min="29" max="29" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="23.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.7109375" customWidth="1"/>
+    <col min="37" max="37" width="20.28515625" customWidth="1"/>
+    <col min="38" max="38" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="14" customFormat="1">
@@ -3683,10 +3669,18 @@
       <c r="AG2" s="31">
         <v>705</v>
       </c>
-      <c r="AH2" s="30"/>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="30"/>
+      <c r="AH2" s="30">
+        <v>123</v>
+      </c>
+      <c r="AI2" s="30">
+        <v>456</v>
+      </c>
+      <c r="AJ2" s="30">
+        <v>789</v>
+      </c>
+      <c r="AK2" s="30">
+        <v>0</v>
+      </c>
       <c r="AL2" s="30"/>
     </row>
     <row r="3" spans="1:38" s="5" customFormat="1" ht="15.75" customHeight="1">
@@ -4285,7 +4279,7 @@
     <sortCondition ref="C2:C7"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL7" xr:uid="{6AA4F54A-41B1-4425-9C81-B6B0EB4AB569}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL7">
       <formula1>"keep_locked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4296,7 +4290,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4304,13 +4298,13 @@
       <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5235,7 +5229,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{AB58DC2F-D10C-4509-A04E-BAF9B4805F01}"/>
+  <autoFilter ref="A1:H1"/>
   <sortState ref="A2:J267">
     <sortCondition ref="C2:C267"/>
     <sortCondition ref="E2:E267"/>
@@ -5245,26 +5239,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8">
+    <row r="1" spans="1:7" ht="30">
       <c r="A1" s="17" t="s">
         <v>23</v>
       </c>
@@ -6218,14 +6212,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G37" xr:uid="{0C1E8CBC-AD96-4338-9B02-9D7DF85F635E}"/>
+  <autoFilter ref="A1:G37"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6236,10 +6230,10 @@
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13" style="26" customWidth="1"/>
-    <col min="2" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="26"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="2" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="26"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33" customHeight="1">
@@ -7136,7 +7130,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U13" xr:uid="{AAD9BEE9-F574-48B8-B79F-6C8F36428352}"/>
+  <autoFilter ref="A1:U13"/>
   <sortState ref="A2:U102">
     <sortCondition ref="B2:B102"/>
   </sortState>
@@ -7146,14 +7140,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7DEC94-3629-421E-B11F-278FCD133C57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="24"/>

</xml_diff>